<commit_message>
adding data as usual
</commit_message>
<xml_diff>
--- a/ParticleSystem_database.xlsx
+++ b/ParticleSystem_database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1525"/>
+  <dimension ref="A1:I1538"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44648,10 +44648,8 @@
       </c>
     </row>
     <row r="1525">
-      <c r="A1525" t="inlineStr">
-        <is>
-          <t>00002585</t>
-        </is>
+      <c r="A1525" t="n">
+        <v>2585</v>
       </c>
       <c r="B1525" t="n">
         <v>0.4</v>
@@ -44675,6 +44673,385 @@
         <v>4026</v>
       </c>
       <c r="I1525" t="n">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="n">
+        <v>2586</v>
+      </c>
+      <c r="B1526" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1526" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1526" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1526" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1526" t="n">
+        <v>300</v>
+      </c>
+      <c r="G1526" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1526" t="n">
+        <v>12037</v>
+      </c>
+      <c r="I1526" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="n">
+        <v>2587</v>
+      </c>
+      <c r="B1527" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1527" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1527" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1527" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1527" t="n">
+        <v>300</v>
+      </c>
+      <c r="G1527" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1527" t="n">
+        <v>12087</v>
+      </c>
+      <c r="I1527" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="n">
+        <v>2588</v>
+      </c>
+      <c r="B1528" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1528" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1528" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1528" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1528" t="n">
+        <v>300</v>
+      </c>
+      <c r="G1528" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1528" t="n">
+        <v>11975</v>
+      </c>
+      <c r="I1528" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="n">
+        <v>2589</v>
+      </c>
+      <c r="B1529" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1529" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1529" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1529" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1529" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1529" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1529" t="n">
+        <v>4023</v>
+      </c>
+      <c r="I1529" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="n">
+        <v>2590</v>
+      </c>
+      <c r="B1530" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C1530" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1530" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1530" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1530" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1530" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1530" t="n">
+        <v>1933</v>
+      </c>
+      <c r="I1530" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="n">
+        <v>2591</v>
+      </c>
+      <c r="B1531" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C1531" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1531" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1531" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1531" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1531" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1531" t="n">
+        <v>6077</v>
+      </c>
+      <c r="I1531" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="n">
+        <v>2592</v>
+      </c>
+      <c r="B1532" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1532" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D1532" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1532" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1532" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1532" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1532" t="n">
+        <v>3981</v>
+      </c>
+      <c r="I1532" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" t="n">
+        <v>2593</v>
+      </c>
+      <c r="B1533" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C1533" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1533" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1533" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1533" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1533" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1533" t="n">
+        <v>6023</v>
+      </c>
+      <c r="I1533" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" t="n">
+        <v>2594</v>
+      </c>
+      <c r="B1534" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C1534" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1534" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E1534" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1534" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1534" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1534" t="n">
+        <v>5932</v>
+      </c>
+      <c r="I1534" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" t="n">
+        <v>2595</v>
+      </c>
+      <c r="B1535" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1535" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1535" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1535" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1535" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1535" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1535" t="n">
+        <v>3941</v>
+      </c>
+      <c r="I1535" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" t="n">
+        <v>2596</v>
+      </c>
+      <c r="B1536" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1536" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1536" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1536" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1536" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1536" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1536" t="n">
+        <v>4048</v>
+      </c>
+      <c r="I1536" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" t="n">
+        <v>2597</v>
+      </c>
+      <c r="B1537" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1537" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D1537" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1537" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1537" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1537" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1537" t="n">
+        <v>4010</v>
+      </c>
+      <c r="I1537" t="n">
+        <v>1e+18</v>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" t="inlineStr">
+        <is>
+          <t>00002598</t>
+        </is>
+      </c>
+      <c r="B1538" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C1538" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D1538" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E1538" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F1538" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1538" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1538" t="n">
+        <v>3941</v>
+      </c>
+      <c r="I1538" t="n">
         <v>5000000</v>
       </c>
     </row>

</xml_diff>